<commit_message>
Improved biplots with Rezek
</commit_message>
<xml_diff>
--- a/old_models/data/Phytoplankton Calculation from Fry 2002.xlsx
+++ b/old_models/data/Phytoplankton Calculation from Fry 2002.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17035\Desktop\New GitHub\Brown-vs-Green\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17035\Desktop\New GitHub\Brown-vs-Green\old_models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396B5287-CCC4-4DF0-8719-0B093009521C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEFF351-8256-44F0-ACBE-50748C6B413F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46575" yWindow="1185" windowWidth="27975" windowHeight="21000" xr2:uid="{0585427B-9D6B-488F-A954-7282565750D8}"/>
+    <workbookView xWindow="105" yWindow="105" windowWidth="10830" windowHeight="21000" xr2:uid="{0585427B-9D6B-488F-A954-7282565750D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
   <si>
     <t>Phytonoplankton N</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>SRS6</t>
+  </si>
+  <si>
+    <t>sd set to 0.5 no variance reported in Fry 2002 so improvised sd</t>
   </si>
 </sst>
 </file>
@@ -461,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDB673B-B810-43CD-A34F-AF38DA79FA71}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,17 +789,17 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>2</v>
       </c>
@@ -809,16 +812,26 @@
       <c r="G36" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>19.5</v>
+      </c>
+      <c r="I36">
+        <f>_xlfn.STDEV.S(H36:H38)</f>
+        <v>3.2532035493238616</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>6</v>
       </c>
       <c r="C37" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -831,12 +844,15 @@
       <c r="F38">
         <v>-24.95</v>
       </c>
-      <c r="G38">
-        <f>STDEVA(B38:C38)</f>
-        <v>0.9192388155425123</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" t="str">
+        <f>I43</f>
+        <v>sd set to 0.5 no variance reported in Fry 2002 so improvised sd</v>
+      </c>
+      <c r="H38">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>20</v>
       </c>
@@ -847,7 +863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <v>6</v>
       </c>
@@ -855,7 +871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -869,16 +885,18 @@
         <v>19.5</v>
       </c>
       <c r="G43">
-        <f>STDEVA(B43:C43)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>2</v>
       </c>
@@ -886,7 +904,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
         <v>6</v>
       </c>
@@ -906,7 +924,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>